<commit_message>
part 2 kind of works. Need to fix leasts
</commit_message>
<xml_diff>
--- a/cs4735/sabinadev/assign2/Matchings.xlsx
+++ b/cs4735/sabinadev/assign2/Matchings.xlsx
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>Color Matching</t>
-  </si>
-  <si>
-    <t>Color Matching</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -47,6 +44,9 @@
   <si>
     <t>Player1</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Texture Matching</t>
   </si>
   <si>
     <t>Texture Matching</t>
@@ -438,7 +438,7 @@
   <dimension ref="A4:G192"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A148" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G185" sqref="G185"/>
+      <selection activeCell="G170" sqref="G170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -454,12 +454,12 @@
   <sheetData>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -468,10 +468,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1402,7 +1402,7 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1412,10 +1412,10 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -2374,7 +2374,7 @@
     </row>
     <row r="102" spans="1:7">
       <c r="A102" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2383,10 +2383,10 @@
     </row>
     <row r="103" spans="1:7">
       <c r="A103" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
@@ -3322,12 +3322,9 @@
     </row>
     <row r="151" spans="1:7">
       <c r="A151" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B151" s="2"/>
-      <c r="C151" s="1"/>
-      <c r="D151" s="1"/>
-      <c r="E151" s="1"/>
     </row>
     <row r="152" spans="1:7">
       <c r="A152" s="1" t="s">
@@ -3348,22 +3345,22 @@
         <v>1</v>
       </c>
       <c r="B153">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C153">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D153">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E153">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F153">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G153">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -3371,22 +3368,22 @@
         <v>2</v>
       </c>
       <c r="B154">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C154">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="D154">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E154">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F154">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G154">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="155" spans="1:7">
@@ -3394,22 +3391,22 @@
         <v>3</v>
       </c>
       <c r="B155">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C155">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D155">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="E155">
+        <v>32</v>
+      </c>
+      <c r="F155">
         <v>36</v>
       </c>
-      <c r="F155">
-        <v>31</v>
-      </c>
       <c r="G155">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="156" spans="1:7">
@@ -3417,22 +3414,22 @@
         <v>4</v>
       </c>
       <c r="B156">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C156">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D156">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E156">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="F156">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="G156">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="157" spans="1:7">
@@ -3443,19 +3440,19 @@
         <v>6</v>
       </c>
       <c r="C157">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D157">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="E157">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="F157">
         <v>31</v>
       </c>
       <c r="G157">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="158" spans="1:7">
@@ -3463,22 +3460,22 @@
         <v>6</v>
       </c>
       <c r="B158">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C158">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D158">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E158">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F158">
         <v>22</v>
       </c>
       <c r="G158">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="159" spans="1:7">
@@ -3486,22 +3483,22 @@
         <v>7</v>
       </c>
       <c r="B159">
+        <v>16</v>
+      </c>
+      <c r="C159">
+        <v>6</v>
+      </c>
+      <c r="D159">
         <v>8</v>
       </c>
-      <c r="C159">
-        <v>40</v>
-      </c>
-      <c r="D159">
-        <v>15</v>
-      </c>
       <c r="E159">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F159">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G159">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="160" spans="1:7">
@@ -3509,22 +3506,22 @@
         <v>8</v>
       </c>
       <c r="B160">
+        <v>16</v>
+      </c>
+      <c r="C160">
         <v>7</v>
       </c>
-      <c r="C160">
-        <v>6</v>
-      </c>
       <c r="D160">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E160">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F160">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="G160">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="161" spans="1:7">
@@ -3535,19 +3532,19 @@
         <v>3</v>
       </c>
       <c r="C161">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D161">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E161">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F161">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G161">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="162" spans="1:7">
@@ -3555,22 +3552,22 @@
         <v>10</v>
       </c>
       <c r="B162">
+        <v>11</v>
+      </c>
+      <c r="C162">
         <v>1</v>
       </c>
-      <c r="C162">
-        <v>3</v>
-      </c>
       <c r="D162">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E162">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F162">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G162">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="163" spans="1:7">
@@ -3578,22 +3575,22 @@
         <v>11</v>
       </c>
       <c r="B163">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C163">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D163">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E163">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F163">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G163">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="164" spans="1:7">
@@ -3601,22 +3598,22 @@
         <v>12</v>
       </c>
       <c r="B164">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C164">
+        <v>5</v>
+      </c>
+      <c r="D164">
         <v>2</v>
       </c>
-      <c r="D164">
-        <v>39</v>
-      </c>
       <c r="E164">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F164">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G164">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="165" spans="1:7">
@@ -3624,22 +3621,22 @@
         <v>13</v>
       </c>
       <c r="B165">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="C165">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D165">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E165">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F165">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="G165">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="166" spans="1:7">
@@ -3647,22 +3644,22 @@
         <v>14</v>
       </c>
       <c r="B166">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C166">
+        <v>25</v>
+      </c>
+      <c r="D166">
         <v>12</v>
       </c>
-      <c r="D166">
-        <v>2</v>
-      </c>
       <c r="E166">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F166">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="G166">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="167" spans="1:7">
@@ -3670,22 +3667,22 @@
         <v>15</v>
       </c>
       <c r="B167">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="C167">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D167">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E167">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F167">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G167">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="168" spans="1:7">
@@ -3693,22 +3690,22 @@
         <v>16</v>
       </c>
       <c r="B168">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C168">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D168">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E168">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F168">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G168">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="169" spans="1:7">
@@ -3716,22 +3713,22 @@
         <v>17</v>
       </c>
       <c r="B169">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C169">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D169">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E169">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F169">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G169">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -3739,22 +3736,22 @@
         <v>18</v>
       </c>
       <c r="B170">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C170">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D170">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E170">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F170">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="G170">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="171" spans="1:7">
@@ -3762,482 +3759,482 @@
         <v>19</v>
       </c>
       <c r="B171">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C171">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D171">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E171">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="F171">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G171">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="172" spans="1:7">
       <c r="A172">
+        <v>19</v>
+      </c>
+      <c r="B172">
         <v>20</v>
       </c>
-      <c r="B172">
-        <v>22</v>
-      </c>
       <c r="C172">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D172">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E172">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F172">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="G172">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="173" spans="1:7">
       <c r="A173">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B173">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C173">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D173">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E173">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F173">
+        <v>9</v>
+      </c>
+      <c r="G173">
         <v>3</v>
-      </c>
-      <c r="G173">
-        <v>13</v>
       </c>
     </row>
     <row r="174" spans="1:7">
       <c r="A174">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B174">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C174">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D174">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E174">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="F174">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G174">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="175" spans="1:7">
       <c r="A175">
+        <v>22</v>
+      </c>
+      <c r="B175">
         <v>23</v>
       </c>
-      <c r="B175">
-        <v>6</v>
-      </c>
       <c r="C175">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D175">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="E175">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="F175">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="G175">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="176" spans="1:7">
       <c r="A176">
+        <v>23</v>
+      </c>
+      <c r="B176">
         <v>24</v>
       </c>
-      <c r="B176">
-        <v>3</v>
-      </c>
       <c r="C176">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D176">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="E176">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F176">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G176">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="177" spans="1:7">
       <c r="A177">
+        <v>24</v>
+      </c>
+      <c r="B177">
+        <v>33</v>
+      </c>
+      <c r="C177">
+        <v>28</v>
+      </c>
+      <c r="D177">
         <v>25</v>
       </c>
-      <c r="B177">
-        <v>28</v>
-      </c>
-      <c r="C177">
-        <v>17</v>
-      </c>
-      <c r="D177">
-        <v>20</v>
-      </c>
       <c r="E177">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="F177">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="G177">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="178" spans="1:7">
       <c r="A178">
+        <v>25</v>
+      </c>
+      <c r="B178">
+        <v>14</v>
+      </c>
+      <c r="C178">
+        <v>5</v>
+      </c>
+      <c r="D178">
+        <v>2</v>
+      </c>
+      <c r="E178">
         <v>26</v>
       </c>
-      <c r="B178">
-        <v>36</v>
-      </c>
-      <c r="C178">
-        <v>18</v>
-      </c>
-      <c r="D178">
-        <v>17</v>
-      </c>
-      <c r="E178">
-        <v>31</v>
-      </c>
       <c r="F178">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G178">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="179" spans="1:7">
       <c r="A179">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B179">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C179">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="D179">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E179">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F179">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G179">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="180" spans="1:7">
       <c r="A180">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B180">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C180">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D180">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E180">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F180">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="G180">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="181" spans="1:7">
       <c r="A181">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B181">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C181">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D181">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E181">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="F181">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G181">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182" spans="1:7">
       <c r="A182">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B182">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C182">
         <v>22</v>
       </c>
       <c r="D182">
+        <v>37</v>
+      </c>
+      <c r="E182">
         <v>13</v>
       </c>
-      <c r="E182">
-        <v>16</v>
-      </c>
       <c r="F182">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="G182">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:7">
       <c r="A183">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B183">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C183">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D183">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="E183">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="F183">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G183">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="184" spans="1:7">
       <c r="A184">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B184">
+        <v>19</v>
+      </c>
+      <c r="C184">
+        <v>17</v>
+      </c>
+      <c r="D184">
         <v>27</v>
       </c>
-      <c r="C184">
-        <v>24</v>
-      </c>
-      <c r="D184">
-        <v>30</v>
-      </c>
       <c r="E184">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F184">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G184">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="185" spans="1:7">
       <c r="A185">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B185">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C185">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D185">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E185">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="F185">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="G185">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="186" spans="1:7">
       <c r="A186">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B186">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C186">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D186">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E186">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F186">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G186">
-        <v>6</v>
+        <v>35</v>
       </c>
     </row>
     <row r="187" spans="1:7">
       <c r="A187">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B187">
+        <v>23</v>
+      </c>
+      <c r="C187">
         <v>22</v>
       </c>
-      <c r="C187">
-        <v>38</v>
-      </c>
       <c r="D187">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E187">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="F187">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G187">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="188" spans="1:7">
       <c r="A188">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B188">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C188">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D188">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E188">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="F188">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G188">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="189" spans="1:7">
       <c r="A189">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B189">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C189">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="D189">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E189">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F189">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G189">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="1:7">
       <c r="A190">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B190">
+        <v>26</v>
+      </c>
+      <c r="C190">
+        <v>30</v>
+      </c>
+      <c r="D190">
         <v>35</v>
       </c>
-      <c r="C190">
-        <v>19</v>
-      </c>
-      <c r="D190">
-        <v>24</v>
-      </c>
       <c r="E190">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F190">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G190">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="191" spans="1:7">
       <c r="A191">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B191">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C191">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D191">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E191">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="F191">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="G191">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="192" spans="1:7">
@@ -4245,22 +4242,22 @@
         <v>40</v>
       </c>
       <c r="B192">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C192">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D192">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="E192">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="F192">
         <v>27</v>
       </c>
       <c r="G192">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>